<commit_message>
Uzupełniony backlog o zaczęte zadania
</commit_message>
<xml_diff>
--- a/Documents/Backlog.xlsx
+++ b/Documents/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hazar\OneDrive\Dokumenty\Pierdoły\Studia\2 semestr AiR\Narzędzia pracy grupowej\WhosThere\WhosThere\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F6D44A-3CBA-46C3-A281-4CEF342B09E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDA6E40-FAF9-44E0-80E3-7942E9AD19B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB39B143-865E-4DD6-BAEF-9CFDD188383C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Backlog WhosThere</t>
   </si>
@@ -43,6 +43,138 @@
   </si>
   <si>
     <t>Czas pracy</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>06.05.2024r.</t>
+  </si>
+  <si>
+    <t>Patryk</t>
+  </si>
+  <si>
+    <t>Naprawa myszki</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>Ukończono</t>
+  </si>
+  <si>
+    <t>Przemek</t>
+  </si>
+  <si>
+    <t>Stworzenie Repozytorium i Projektu</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Kamil</t>
+  </si>
+  <si>
+    <t>Robienie zdjęć: zaprogramowanie kamery</t>
+  </si>
+  <si>
+    <t>75 min</t>
+  </si>
+  <si>
+    <t>09.05 - 10.05.24r.</t>
+  </si>
+  <si>
+    <t>08.05 - 10.05.24r.</t>
+  </si>
+  <si>
+    <t>Justyna</t>
+  </si>
+  <si>
+    <t>Robienie zdjęć: Stworzenie warunku sprawdzającego if</t>
+  </si>
+  <si>
+    <t>80 min</t>
+  </si>
+  <si>
+    <t>11.05.2024r.</t>
+  </si>
+  <si>
+    <t>trening: enkodowanie</t>
+  </si>
+  <si>
+    <t>120 min</t>
+  </si>
+  <si>
+    <t>main: Odczytanie danych z pliku .yaml</t>
+  </si>
+  <si>
+    <t>11.05 - 12.05.24r.</t>
+  </si>
+  <si>
+    <t>290 min</t>
+  </si>
+  <si>
+    <t>12.05.2024r.</t>
+  </si>
+  <si>
+    <t>main: szacowanie rozpoznania</t>
+  </si>
+  <si>
+    <t>100 min</t>
+  </si>
+  <si>
+    <t>main: złączenie całości</t>
+  </si>
+  <si>
+    <t>13.05.2024r.</t>
+  </si>
+  <si>
+    <t>70 min</t>
+  </si>
+  <si>
+    <t>Zapoznać się z biblioteką python tkinter</t>
+  </si>
+  <si>
+    <t>Wszyscy</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>W trakcie</t>
+  </si>
+  <si>
+    <t>Zapoznać się z biblioteką python CV2</t>
+  </si>
+  <si>
+    <t>Zapoznać się z biblioteką python face_recognition</t>
+  </si>
+  <si>
+    <t>take_photo: implementacja przycisków wyjścia i zapisu</t>
+  </si>
+  <si>
+    <t>55 min</t>
+  </si>
+  <si>
+    <t>19.05 -</t>
+  </si>
+  <si>
+    <t>Dodanie backlogu</t>
+  </si>
+  <si>
+    <t>22.05.2024r.</t>
+  </si>
+  <si>
+    <t>35 min</t>
+  </si>
+  <si>
+    <t>take_photo: implementacja przycisku usuwania</t>
+  </si>
+  <si>
+    <t>20.05 -</t>
+  </si>
+  <si>
+    <t>Do zrobienia</t>
   </si>
 </sst>
 </file>
@@ -59,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,6 +201,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -85,16 +223,119 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -404,18 +645,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886C42E0-FDBA-4042-95B4-E83169C6C7B4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="15.77734375" customWidth="1"/>
+    <col min="1" max="6" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,28 +664,333 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:F3">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="W trakcie">
+      <formula>NOT(ISERROR(SEARCH("W trakcie",A3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="W trakcie">
+      <formula>NOT(ISERROR(SEARCH("W trakcie",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Ukończono">
+      <formula>NOT(ISERROR(SEARCH("Ukończono",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Do zrobienia">
+      <formula>NOT(ISERROR(SEARCH("Do zrobienia",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Dodanie aktywności do backlogu
</commit_message>
<xml_diff>
--- a/Documents/Backlog.xlsx
+++ b/Documents/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konpf\Desktop\AGH AiR\Semestr 2\NPG\Who's there\WhosThere\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F207743C-6867-4282-BE93-3FD5D53CBE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085A6862-F4DD-422E-A4B1-C0982825E872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-990" windowWidth="25440" windowHeight="15390" xr2:uid="{FB39B143-865E-4DD6-BAEF-9CFDD188383C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB39B143-865E-4DD6-BAEF-9CFDD188383C}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="44">
   <si>
     <t>Backlog WhosThere</t>
   </si>
@@ -2728,8 +2728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886C42E0-FDBA-4042-95B4-E83169C6C7B4}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="92" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3342,15 +3342,43 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>45443</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>45443</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>35</v>
+      </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Dodano aktywność w backlogu
</commit_message>
<xml_diff>
--- a/Documents/Backlog.xlsx
+++ b/Documents/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konpf\Desktop\AGH AiR\Semestr 2\NPG\Who's there\WhosThere\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7053806-7C3C-49A3-8E9E-C99F466D3038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD904AEA-8515-4A06-B6C6-91FDB3EA2D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB39B143-865E-4DD6-BAEF-9CFDD188383C}"/>
   </bookViews>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -246,8 +246,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -3347,22 +3345,22 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+      <c r="A26" s="1">
         <v>45441</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26">
         <v>3</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26">
         <v>120</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="4"/>

</xml_diff>

<commit_message>
Wykonanie zadań oraz aktualizacja dokumentacji
</commit_message>
<xml_diff>
--- a/Documents/Backlog.xlsx
+++ b/Documents/Backlog.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konpf\Desktop\AGH AiR\Semestr 2\NPG\Who's there\WhosThere\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT_REPOS\WhosThere\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35DBCDE-64D9-4CD7-9A8E-03FC118B5A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296120BA-5915-4A8D-B303-99E5F59DB4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB39B143-865E-4DD6-BAEF-9CFDD188383C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FB39B143-865E-4DD6-BAEF-9CFDD188383C}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t>Backlog WhosThere</t>
   </si>
@@ -189,6 +178,15 @@
   </si>
   <si>
     <t>ogół prac</t>
+  </si>
+  <si>
+    <t>main: dodać funkcjonalność przycisku do wychodzenia z programu</t>
+  </si>
+  <si>
+    <t>trening: dodanie graficznego interfejsu</t>
+  </si>
+  <si>
+    <t>3 sprint</t>
   </si>
 </sst>
 </file>
@@ -266,7 +264,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -326,7 +324,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -846,7 +844,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1331,7 +1329,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1453,7 +1451,7 @@
                   <c:v>5.916666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.833333333333333</c:v>
+                  <c:v>8.8333333333333339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3489,8 +3487,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{56F8B267-4195-4B64-A121-BDEF55206FFC}" name="Tabela3" displayName="Tabela3" ref="A2:F34" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A2:F34" xr:uid="{56F8B267-4195-4B64-A121-BDEF55206FFC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{56F8B267-4195-4B64-A121-BDEF55206FFC}" name="Tabela3" displayName="Tabela3" ref="A2:F36" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A2:F36" xr:uid="{56F8B267-4195-4B64-A121-BDEF55206FFC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F22">
     <sortCondition ref="A2:A22"/>
   </sortState>
@@ -3507,9 +3505,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office 2013–2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3547,7 +3545,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office 2013–2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3653,7 +3651,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office 2013–2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3795,7 +3793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3803,38 +3801,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886C42E0-FDBA-4042-95B4-E83169C6C7B4}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="92" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="92" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5546875" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" customWidth="1"/>
-    <col min="17" max="17" width="8.44140625" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3856,13 +3855,19 @@
         <v>39</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="S1" t="s">
         <v>39</v>
       </c>
+      <c r="V1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45418</v>
       </c>
@@ -3919,8 +3924,12 @@
         <v>13</v>
       </c>
       <c r="S3" s="3"/>
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45418</v>
       </c>
@@ -3957,8 +3966,12 @@
         <v>6</v>
       </c>
       <c r="S4" s="3"/>
+      <c r="V4" t="s">
+        <v>6</v>
+      </c>
+      <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45418</v>
       </c>
@@ -3995,8 +4008,12 @@
         <v>11</v>
       </c>
       <c r="S5" s="3"/>
+      <c r="V5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45418</v>
       </c>
@@ -4033,8 +4050,12 @@
         <v>9</v>
       </c>
       <c r="S6" s="3"/>
+      <c r="V6" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45418</v>
       </c>
@@ -4055,7 +4076,7 @@
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45422</v>
       </c>
@@ -4075,7 +4096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45422</v>
       </c>
@@ -4095,7 +4116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45423</v>
       </c>
@@ -4115,7 +4136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45424</v>
       </c>
@@ -4135,7 +4156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45424</v>
       </c>
@@ -4155,7 +4176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45425</v>
       </c>
@@ -4175,7 +4196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45430</v>
       </c>
@@ -4195,7 +4216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45430</v>
       </c>
@@ -4215,7 +4236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45431</v>
       </c>
@@ -4235,7 +4256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45432</v>
       </c>
@@ -4255,7 +4276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45433</v>
       </c>
@@ -4275,7 +4296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45434</v>
       </c>
@@ -4295,7 +4316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45435</v>
       </c>
@@ -4315,7 +4336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45436</v>
       </c>
@@ -4335,7 +4356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45436</v>
       </c>
@@ -4355,7 +4376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45436</v>
       </c>
@@ -4375,7 +4396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45441</v>
       </c>
@@ -4395,7 +4416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45442</v>
       </c>
@@ -4418,7 +4439,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45441</v>
       </c>
@@ -4439,7 +4460,7 @@
       </c>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45443</v>
       </c>
@@ -4459,7 +4480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45443</v>
       </c>
@@ -4479,7 +4500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45448</v>
       </c>
@@ -4502,7 +4523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45448</v>
       </c>
@@ -4522,7 +4543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45451</v>
       </c>
@@ -4545,11 +4566,11 @@
         <v>13</v>
       </c>
       <c r="I31">
-        <f>SUMIF(B6:B34,H3,E6:E34)/60</f>
+        <f>SUMIF(B6:B34,H3,E6:E107)/60</f>
         <v>6.583333333333333</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45451</v>
       </c>
@@ -4572,11 +4593,11 @@
         <v>6</v>
       </c>
       <c r="I32">
-        <f t="shared" ref="I32:I34" si="1">SUMIF(B7:B35,H4,E7:E35)/60</f>
+        <f>SUMIF(B7:B35,H4,E7:E107)/60</f>
         <v>15.583333333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45452</v>
       </c>
@@ -4599,11 +4620,11 @@
         <v>11</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
+        <f>SUMIF(B8:B36,H5,E8:E107)/60</f>
         <v>5.916666666666667</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45452</v>
       </c>
@@ -4626,8 +4647,48 @@
         <v>9</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
-        <v>6.833333333333333</v>
+        <f>SUMIF(B9:B37,H6,E9:E107)/60</f>
+        <v>8.8333333333333339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45452</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>60</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45452</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>60</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>